<commit_message>
the documents are set now
</commit_message>
<xml_diff>
--- a/doc/MasterQuad2015_BusLoad_estimation.xlsx
+++ b/doc/MasterQuad2015_BusLoad_estimation.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agrawal\work\workspace\helikopter\helikopter-raspberry\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="576" yWindow="120" windowWidth="33348" windowHeight="15336"/>
+    <workbookView xWindow="570" yWindow="120" windowWidth="33345" windowHeight="15330"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -693,14 +698,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -738,9 +746,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,7 +783,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -810,7 +818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -989,26 +997,26 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" customWidth="1"/>
-    <col min="12" max="12" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
@@ -1022,8 +1030,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>26</v>
       </c>
@@ -1052,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -1077,15 +1085,15 @@
         <v>1</v>
       </c>
       <c r="H4" s="11">
-        <f>D4*E4*G4</f>
+        <f t="shared" ref="H4:H12" si="0">D4*E4*G4</f>
         <v>3200</v>
       </c>
       <c r="I4" s="31">
-        <f>H4*$K$16</f>
+        <f t="shared" ref="I4:I12" si="1">H4*$K$16</f>
         <v>32000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
@@ -1097,29 +1105,29 @@
         <v>24</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5" si="0">B5*C5</f>
+        <f t="shared" ref="D5" si="2">B5*C5</f>
         <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>800</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">D5*E5</f>
+        <f t="shared" ref="F5:F12" si="3">D5*E5</f>
         <v>19200</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
       </c>
       <c r="H5" s="8">
-        <f>D5*E5*G5</f>
+        <f t="shared" si="0"/>
         <v>19200</v>
       </c>
       <c r="I5" s="32">
-        <f>H5*$K$16</f>
+        <f t="shared" si="1"/>
         <v>192000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
@@ -1131,29 +1139,29 @@
         <v>24</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6" si="2">B6*C6</f>
+        <f t="shared" ref="D6" si="4">B6*C6</f>
         <v>24</v>
       </c>
       <c r="E6" s="3">
         <v>100</v>
       </c>
       <c r="F6" s="3">
+        <f t="shared" si="3"/>
+        <v>2400</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="I6" s="32">
         <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <f>D6*E6*G6</f>
-        <v>2400</v>
-      </c>
-      <c r="I6" s="32">
-        <f>H6*$K$16</f>
         <v>24000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
@@ -1172,22 +1180,22 @@
         <v>800</v>
       </c>
       <c r="F7" s="3">
+        <f t="shared" si="3"/>
+        <v>19200</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>19200</v>
+      </c>
+      <c r="I7" s="32">
         <f t="shared" si="1"/>
-        <v>19200</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <f>D7*E7*G7</f>
-        <v>19200</v>
-      </c>
-      <c r="I7" s="32">
-        <f>H7*$K$16</f>
         <v>192000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
@@ -1206,22 +1214,22 @@
         <v>25</v>
       </c>
       <c r="F8" s="3">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="I8" s="32">
         <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <f>D8*E8*G8</f>
-        <v>300</v>
-      </c>
-      <c r="I8" s="32">
-        <f>H8*$K$16</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -1240,22 +1248,22 @@
         <v>50</v>
       </c>
       <c r="F9" s="3">
+        <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="I9" s="32">
         <f t="shared" si="1"/>
-        <v>1800</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <f>D9*E9*G9</f>
-        <v>1800</v>
-      </c>
-      <c r="I9" s="32">
-        <f>H9*$K$16</f>
         <v>18000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
@@ -1273,62 +1281,62 @@
         <v>10</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="G10" s="8">
         <v>8</v>
       </c>
       <c r="H10" s="8">
-        <f>D10*E10*G10</f>
+        <f t="shared" si="0"/>
         <v>720</v>
       </c>
       <c r="I10" s="32">
-        <f>H10*$K$16</f>
+        <f t="shared" si="1"/>
         <v>7200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
-        <f>D11*E11*G11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="32">
-        <f>H11*$K$16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9">
-        <f>D12*E12*G12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="33">
-        <f>H12*$K$16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>9</v>
       </c>
@@ -1362,7 +1370,7 @@
         <v>468200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
@@ -1373,7 +1381,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -1391,7 +1399,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>21</v>
       </c>
@@ -1414,19 +1422,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
       <c r="L17" s="39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="95.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="95.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="1"/>
       <c r="L18" s="38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>3</v>
       </c>
@@ -1480,15 +1488,15 @@
         <v>1</v>
       </c>
       <c r="H20" s="2">
-        <f>D20*E20*G20</f>
+        <f t="shared" ref="H20:H28" si="5">D20*E20*G20</f>
         <v>3200</v>
       </c>
       <c r="I20" s="31">
-        <f>H20*$K$16</f>
+        <f t="shared" ref="I20:I28" si="6">H20*$K$16</f>
         <v>32000</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>14</v>
       </c>
@@ -1500,29 +1508,29 @@
         <v>9</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" ref="D21" si="3">B21*C21</f>
+        <f t="shared" ref="D21" si="7">B21*C21</f>
         <v>9</v>
       </c>
       <c r="E21" s="8">
         <v>800</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="4">D21*E21</f>
+        <f t="shared" ref="F21:F28" si="8">D21*E21</f>
         <v>7200</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
       </c>
       <c r="H21" s="3">
-        <f>D21*E21*G21</f>
+        <f t="shared" si="5"/>
         <v>7200</v>
       </c>
       <c r="I21" s="32">
-        <f>H21*$K$16</f>
+        <f t="shared" si="6"/>
         <v>72000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>15</v>
       </c>
@@ -1534,29 +1542,29 @@
         <v>9</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" ref="D22" si="5">B22*C22</f>
+        <f t="shared" ref="D22" si="9">B22*C22</f>
         <v>9</v>
       </c>
       <c r="E22" s="8">
         <v>100</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>900</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
       </c>
       <c r="H22" s="3">
-        <f>D22*E22*G22</f>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="I22" s="32">
-        <f>H22*$K$16</f>
+        <f t="shared" si="6"/>
         <v>9000</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>4</v>
       </c>
@@ -1575,22 +1583,22 @@
         <v>800</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7200</v>
       </c>
       <c r="G23" s="10">
         <v>1</v>
       </c>
       <c r="H23" s="3">
-        <f>D23*E23*G23</f>
+        <f t="shared" si="5"/>
         <v>7200</v>
       </c>
       <c r="I23" s="32">
-        <f>H23*$K$16</f>
+        <f t="shared" si="6"/>
         <v>72000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>5</v>
       </c>
@@ -1609,22 +1617,22 @@
         <v>25</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
       </c>
       <c r="H24" s="3">
-        <f>D24*E24*G24</f>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="I24" s="32">
-        <f>H24*$K$16</f>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>6</v>
       </c>
@@ -1643,22 +1651,22 @@
         <v>50</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1800</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
       </c>
       <c r="H25" s="3">
-        <f>D25*E25*G25</f>
+        <f t="shared" si="5"/>
         <v>1800</v>
       </c>
       <c r="I25" s="32">
-        <f>H25*$K$16</f>
+        <f t="shared" si="6"/>
         <v>18000</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>13</v>
       </c>
@@ -1676,62 +1684,62 @@
         <v>10</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
       <c r="G26" s="10">
         <v>8</v>
       </c>
       <c r="H26" s="3">
-        <f>D26*E26*G26</f>
+        <f t="shared" si="5"/>
         <v>720</v>
       </c>
       <c r="I26" s="32">
-        <f>H26*$K$16</f>
+        <f t="shared" si="6"/>
         <v>7200</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="8"/>
       <c r="F27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="3">
-        <f>D27*E27*G27</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I27" s="32">
-        <f>H27*$K$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="9"/>
       <c r="F28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="5">
-        <f>D28*E28*G28</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I28" s="33">
-        <f>H28*$K$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>9</v>
       </c>
@@ -1765,7 +1773,7 @@
         <v>211700</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -1776,7 +1784,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="23"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -1791,7 +1799,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
         <v>21</v>
       </c>
@@ -1811,7 +1819,7 @@
         <v>0.52925</v>
       </c>
     </row>
-    <row r="36" ht="87.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="87.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1825,7 +1833,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1837,7 +1845,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>